<commit_message>
redid script and added comments
</commit_message>
<xml_diff>
--- a/synuclein_inclusion_biogenesis_2024/image_analysis/mitophagy/72425_SUMMARY.xlsx
+++ b/synuclein_inclusion_biogenesis_2024/image_analysis/mitophagy/72425_SUMMARY.xlsx
@@ -571,7 +571,7 @@
         <v>3</v>
       </c>
       <c r="E7" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
@@ -761,7 +761,7 @@
         <v>3</v>
       </c>
       <c r="E17" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="18">
@@ -1198,7 +1198,7 @@
         <v>4</v>
       </c>
       <c r="E40" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41">
@@ -1331,7 +1331,7 @@
         <v>1</v>
       </c>
       <c r="E47" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="48">
@@ -1464,7 +1464,7 @@
         <v>1</v>
       </c>
       <c r="E54" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="55">
@@ -1673,7 +1673,7 @@
         <v>2</v>
       </c>
       <c r="E65" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="66">
@@ -1996,7 +1996,7 @@
         <v>1</v>
       </c>
       <c r="E82" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83">
@@ -2072,7 +2072,7 @@
         <v>1</v>
       </c>
       <c r="E86" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="87">
@@ -2319,7 +2319,7 @@
         <v>1</v>
       </c>
       <c r="E99" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100">
@@ -2395,7 +2395,7 @@
         <v>2</v>
       </c>
       <c r="E103" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="104">
@@ -2604,7 +2604,7 @@
         <v>4</v>
       </c>
       <c r="E114" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="115">
@@ -2756,7 +2756,7 @@
         <v>1</v>
       </c>
       <c r="E122" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123">
@@ -2908,7 +2908,7 @@
         <v>1</v>
       </c>
       <c r="E130" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131">

</xml_diff>